<commit_message>
Script Flow Change Assessment 2 Commit - Sundar
</commit_message>
<xml_diff>
--- a/SeleniumCaseStudy/src/test/resources/Resources/TestData.xlsx
+++ b/SeleniumCaseStudy/src/test/resources/Resources/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SeleniumCaseStudy\SeleniumCaseStudy\src\test\resources\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SeleniumStudy\SeleniumCaseStudy\src\test\resources\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Olay Registration and Sign Single Script developed.
</commit_message>
<xml_diff>
--- a/SeleniumCaseStudy/src/test/resources/Resources/TestData.xlsx
+++ b/SeleniumCaseStudy/src/test/resources/Resources/TestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
   <si>
     <t>Browser</t>
   </si>
@@ -132,21 +132,12 @@
     <t>https://www.olay.co.uk/en-gb</t>
   </si>
   <si>
-    <t>ChinaPassword</t>
-  </si>
-  <si>
     <t>pLMOKN123@456</t>
   </si>
   <si>
-    <t>FirstNameChina</t>
-  </si>
-  <si>
     <t>Corona</t>
   </si>
   <si>
-    <t>LastNameChina</t>
-  </si>
-  <si>
     <t>ChinaAddress</t>
   </si>
   <si>
@@ -204,12 +195,6 @@
     <t>Hegde</t>
   </si>
   <si>
-    <t>InvalidPasswordErrMsg</t>
-  </si>
-  <si>
-    <t>The email and password combination you entered is incorrect. Please try again, or click the link below to create an account.</t>
-  </si>
-  <si>
     <t>PasswordRecoveryMail</t>
   </si>
   <si>
@@ -232,6 +217,15 @@
   </si>
   <si>
     <t>7402376699</t>
+  </si>
+  <si>
+    <t>OlayPassword</t>
+  </si>
+  <si>
+    <t>FirstNameOlay</t>
+  </si>
+  <si>
+    <t>LastNameOlay</t>
   </si>
 </sst>
 </file>
@@ -574,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,7 +631,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -733,138 +727,130 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>